<commit_message>
New benchmark update - implemented new stage distribution
</commit_message>
<xml_diff>
--- a/SEER analysis/Mortality2004+.xlsx
+++ b/SEER analysis/Mortality2004+.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janek/Documents/GitHub/CMOSTv2/SEER analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FCD9A3-2A8F-A84C-ABB9-9C705522B24A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAB39CD-4C9C-D542-953E-20D3D5C4923C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9120" yWindow="-18560" windowWidth="27660" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7060" yWindow="8260" windowWidth="27660" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Age recode with &lt;1 year olds</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>Male and female</t>
+  </si>
+  <si>
+    <t>(0,4]</t>
+  </si>
+  <si>
+    <t>(4,9]</t>
+  </si>
+  <si>
+    <t>(9,14]</t>
   </si>
 </sst>
 </file>
@@ -171,7 +180,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sheet 1'!$A$2:$A$16</c:f>
+              <c:f>'Sheet 1'!$A$5:$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -224,7 +233,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet 1'!$B$2:$B$16</c:f>
+              <c:f>'Sheet 1'!$B$5:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -303,7 +312,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sheet 1'!$A$2:$A$16</c:f>
+              <c:f>'Sheet 1'!$A$5:$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -356,7 +365,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet 1'!$C$2:$C$16</c:f>
+              <c:f>'Sheet 1'!$C$5:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -435,7 +444,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sheet 1'!$A$2:$A$16</c:f>
+              <c:f>'Sheet 1'!$A$5:$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -488,7 +497,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet 1'!$D$2:$D$16</c:f>
+              <c:f>'Sheet 1'!$D$5:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1426,13 +1435,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1740,10 +1749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1769,7 +1778,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1783,197 +1792,239 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>2.1</v>
+        <v>0.2</v>
       </c>
       <c r="C6">
-        <v>2.4</v>
+        <v>0.2</v>
       </c>
       <c r="D6">
-        <v>1.9</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>4.2</v>
+        <v>0.5</v>
       </c>
       <c r="C7">
-        <v>4.5999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="D7">
-        <v>3.8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>7.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C8">
-        <v>8.9</v>
+        <v>1.2</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>13.7</v>
+        <v>2.1</v>
       </c>
       <c r="C9">
-        <v>15.9</v>
+        <v>2.4</v>
       </c>
       <c r="D9">
-        <v>11.5</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>20.8</v>
+        <v>4.2</v>
       </c>
       <c r="C10">
-        <v>25.3</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D10">
-        <v>16.5</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>30.9</v>
+        <v>7.9</v>
       </c>
       <c r="C11">
-        <v>38.5</v>
+        <v>8.9</v>
       </c>
       <c r="D11">
-        <v>23.9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>43.8</v>
+        <v>13.7</v>
       </c>
       <c r="C12">
-        <v>54.8</v>
+        <v>15.9</v>
       </c>
       <c r="D12">
-        <v>34</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>20.8</v>
       </c>
       <c r="C13">
-        <v>78.099999999999994</v>
+        <v>25.3</v>
       </c>
       <c r="D13">
-        <v>50.4</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>89.8</v>
+        <v>30.9</v>
       </c>
       <c r="C14">
-        <v>109.2</v>
+        <v>38.5</v>
       </c>
       <c r="D14">
-        <v>74.900000000000006</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>127.2</v>
+        <v>43.8</v>
       </c>
       <c r="C15">
-        <v>152.4</v>
+        <v>54.8</v>
       </c>
       <c r="D15">
-        <v>110.3</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>63</v>
+      </c>
+      <c r="C16">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="D16">
+        <v>50.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>89.8</v>
+      </c>
+      <c r="C17">
+        <v>109.2</v>
+      </c>
+      <c r="D17">
+        <v>74.900000000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>127.2</v>
+      </c>
+      <c r="C18">
+        <v>152.4</v>
+      </c>
+      <c r="D18">
+        <v>110.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B16">
+      <c r="B19">
         <v>198</v>
       </c>
-      <c r="C16">
+      <c r="C19">
         <v>226.4</v>
       </c>
-      <c r="D16">
+      <c r="D19">
         <v>184.2</v>
       </c>
     </row>

</xml_diff>